<commit_message>
Updates misspelled Manhica in Form B choices
</commit_message>
<xml_diff>
--- a/Hluvukani_B_registrar_pessoas/Hluvukani_B_registrar_pessoas-media/Hluvukani_B_registrar_pessoas.xlsx
+++ b/Hluvukani_B_registrar_pessoas/Hluvukani_B_registrar_pessoas-media/Hluvukani_B_registrar_pessoas.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Work_Terra_Firma_Lda\Projects\On_Indufor_Illovo_Moz\Work\ODK\New May 2017\Hluvukani_B_registrar_pessoas\Hluvukani_B_registrar_pessoas-media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\illovo\ODK Forms\hluvukani-odk-forms\Hluvukani_B_registrar_pessoas\Hluvukani_B_registrar_pessoas-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -578,9 +578,6 @@
     <t>E_Palmeira_3</t>
   </si>
   <si>
-    <t>F_Manhiça_Municipality</t>
-  </si>
-  <si>
     <t>J_Munguine_South</t>
   </si>
   <si>
@@ -800,14 +797,24 @@
 O técnico pode usar o formulário para capturar informação sobre cada pessoa, incluindo a foto e assinatura digital.
 Por favor deslizar para a frente para continuar.</t>
   </si>
+  <si>
+    <t>F_Manhica_Municipality</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -984,344 +991,347 @@
   </borders>
   <cellStyleXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="233" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
@@ -1992,7 +2002,7 @@
         <v>60</v>
       </c>
       <c r="M4" s="42" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="42" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
@@ -2003,7 +2013,7 @@
         <v>38</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I5" s="46"/>
     </row>
@@ -2015,7 +2025,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>23</v>
@@ -2083,10 +2093,10 @@
         <v>24</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L10" s="46" t="s">
         <v>34</v>
@@ -2097,16 +2107,16 @@
         <v>32</v>
       </c>
       <c r="B11" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="H11" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="I11" s="46" t="s">
         <v>193</v>
-      </c>
-      <c r="I11" s="46" t="s">
-        <v>194</v>
       </c>
       <c r="J11" s="46" t="s">
         <v>23</v>
@@ -2117,16 +2127,16 @@
         <v>32</v>
       </c>
       <c r="B12" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C12" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="C12" s="46" t="s">
-        <v>196</v>
-      </c>
       <c r="H12" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="I12" s="46" t="s">
         <v>193</v>
-      </c>
-      <c r="I12" s="46" t="s">
-        <v>194</v>
       </c>
       <c r="J12" s="46" t="s">
         <v>23</v>
@@ -2134,13 +2144,13 @@
     </row>
     <row r="13" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="C13" s="46" t="s">
         <v>198</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>199</v>
       </c>
       <c r="I13" s="46"/>
       <c r="J13" s="42" t="s">
@@ -2152,13 +2162,13 @@
     </row>
     <row r="14" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="C14" s="46" t="s">
         <v>201</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>202</v>
       </c>
       <c r="I14" s="46"/>
       <c r="J14" s="42" t="s">
@@ -2178,19 +2188,19 @@
     </row>
     <row r="16" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="C16" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="C16" s="46" t="s">
-        <v>205</v>
-      </c>
       <c r="H16" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="I16" s="46" t="s">
         <v>193</v>
-      </c>
-      <c r="I16" s="46" t="s">
-        <v>194</v>
       </c>
       <c r="L16" s="42" t="s">
         <v>43</v>
@@ -2201,13 +2211,13 @@
         <v>32</v>
       </c>
       <c r="B17" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="G17" s="42" t="s">
         <v>207</v>
-      </c>
-      <c r="G17" s="42" t="s">
-        <v>208</v>
       </c>
       <c r="H17" s="46"/>
       <c r="I17" s="46"/>
@@ -2217,10 +2227,10 @@
         <v>24</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I18" s="46"/>
       <c r="L18" s="42" t="s">
@@ -2232,19 +2242,19 @@
         <v>32</v>
       </c>
       <c r="B19" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="C19" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="H19" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="I19" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="H19" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="I19" s="46" t="s">
+      <c r="K19" s="42" t="s">
         <v>212</v>
-      </c>
-      <c r="K19" s="42" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -2252,16 +2262,16 @@
         <v>32</v>
       </c>
       <c r="B20" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="C20" s="46" t="s">
-        <v>215</v>
-      </c>
       <c r="H20" s="46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I20" s="46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
@@ -2275,10 +2285,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="C22" s="42" t="s">
         <v>216</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>217</v>
       </c>
       <c r="I22" s="46"/>
       <c r="J22" s="42" t="s">
@@ -2293,13 +2303,13 @@
         <v>17</v>
       </c>
       <c r="B23" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="C23" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="G23" s="42" t="s">
         <v>219</v>
-      </c>
-      <c r="G23" s="42" t="s">
-        <v>220</v>
       </c>
       <c r="I23" s="46"/>
       <c r="L23" s="42" t="s">
@@ -2308,16 +2318,16 @@
     </row>
     <row r="24" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="C24" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="G24" s="42" t="s">
         <v>223</v>
-      </c>
-      <c r="G24" s="42" t="s">
-        <v>224</v>
       </c>
       <c r="I24" s="46"/>
       <c r="L24" s="42" t="s">
@@ -2329,10 +2339,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L25" s="46" t="s">
         <v>34</v>
@@ -2340,13 +2350,13 @@
     </row>
     <row r="26" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="B26" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="C26" s="46" t="s">
         <v>227</v>
-      </c>
-      <c r="C26" s="46" t="s">
-        <v>228</v>
       </c>
       <c r="J26" s="46" t="s">
         <v>23</v>
@@ -2360,16 +2370,16 @@
         <v>32</v>
       </c>
       <c r="B27" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="C27" s="46" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="H27" s="46" t="s">
         <v>230</v>
       </c>
-      <c r="H27" s="46" t="s">
+      <c r="I27" s="46" t="s">
         <v>231</v>
-      </c>
-      <c r="I27" s="46" t="s">
-        <v>232</v>
       </c>
       <c r="J27" s="46" t="s">
         <v>23</v>
@@ -2380,16 +2390,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="46" t="s">
         <v>233</v>
       </c>
-      <c r="C28" s="46" t="s">
-        <v>234</v>
-      </c>
       <c r="H28" s="46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I28" s="46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
@@ -2397,10 +2407,10 @@
         <v>17</v>
       </c>
       <c r="B29" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C29" s="46" t="s">
         <v>235</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>236</v>
       </c>
       <c r="L29" s="42" t="s">
         <v>36</v>
@@ -2411,10 +2421,10 @@
         <v>17</v>
       </c>
       <c r="B30" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C30" s="46" t="s">
         <v>237</v>
-      </c>
-      <c r="C30" s="46" t="s">
-        <v>238</v>
       </c>
       <c r="L30" s="42" t="s">
         <v>36</v>
@@ -2425,10 +2435,10 @@
         <v>21</v>
       </c>
       <c r="B31" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="C31" s="46" t="s">
         <v>239</v>
-      </c>
-      <c r="C31" s="46" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
@@ -2442,10 +2452,10 @@
         <v>33</v>
       </c>
       <c r="B33" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="C33" s="46" t="s">
         <v>241</v>
-      </c>
-      <c r="C33" s="46" t="s">
-        <v>242</v>
       </c>
       <c r="J33" s="46" t="s">
         <v>23</v>
@@ -2456,10 +2466,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J34" s="46" t="s">
         <v>23</v>
@@ -2470,33 +2480,33 @@
         <v>33</v>
       </c>
       <c r="B35" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="C35" s="46" t="s">
         <v>243</v>
-      </c>
-      <c r="C35" s="46" t="s">
-        <v>244</v>
       </c>
       <c r="J35" s="46" t="s">
         <v>23</v>
       </c>
       <c r="L35" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
+        <v>251</v>
+      </c>
+      <c r="B36" s="47" t="s">
         <v>252</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="C36" s="46" t="s">
+        <v>254</v>
+      </c>
+      <c r="H36" s="46" t="s">
+        <v>250</v>
+      </c>
+      <c r="L36" s="46" t="s">
         <v>253</v>
-      </c>
-      <c r="C36" s="46" t="s">
-        <v>255</v>
-      </c>
-      <c r="H36" s="46" t="s">
-        <v>251</v>
-      </c>
-      <c r="L36" s="46" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2518,11 +2528,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,8 +2860,8 @@
       <c r="A29" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="50" t="s">
-        <v>184</v>
+      <c r="B29" s="51" t="s">
+        <v>256</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>79</v>
@@ -2911,7 +2921,7 @@
         <v>73</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>80</v>
@@ -2926,7 +2936,7 @@
         <v>73</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C34" s="28" t="s">
         <v>81</v>
@@ -3481,8 +3491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3516,10 +3526,10 @@
         <v>84</v>
       </c>
       <c r="C2" s="6">
-        <v>201705141</v>
+        <v>201708161</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Form B amended to widen constraint and Form D amended to add party_id
</commit_message>
<xml_diff>
--- a/Hluvukani_B_registrar_pessoas/Hluvukani_B_registrar_pessoas-media/Hluvukani_B_registrar_pessoas.xlsx
+++ b/Hluvukani_B_registrar_pessoas/Hluvukani_B_registrar_pessoas-media/Hluvukani_B_registrar_pessoas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">choices!$A$1:$C$18</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -602,9 +602,6 @@
     <t>Qual é o apelido da pessoa?</t>
   </si>
   <si>
-    <t>regex(., "^[a-zA-Z0-9. _-éáíóãõúçâê]{1,25}$")</t>
-  </si>
-  <si>
     <t>Resposta invalida - Os campos de apelido, nome e profissão não podiam incluir um novo paragrafo. Faça a favor de eliminar qualquer linha adicional.</t>
   </si>
   <si>
@@ -800,14 +797,24 @@
   <si>
     <t>F_Manhica_Municipality</t>
   </si>
+  <si>
+    <t>regex(., "^[a-zA-Z0-9. _-éáíóãõúçâôàèê]{1,75}$")</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -991,351 +998,352 @@
   </borders>
   <cellStyleXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="233" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="236">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1571,9 +1579,9 @@
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="233"/>
-    <cellStyle name="Normal 3 2" xfId="234"/>
-    <cellStyle name="Normal 3 2 2" xfId="235"/>
+    <cellStyle name="Normal 2" xfId="233" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Normal 3 2" xfId="234" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1909,14 +1917,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,7 +2021,7 @@
         <v>38</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I5" s="46"/>
     </row>
@@ -2093,7 +2101,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>189</v>
@@ -2112,11 +2120,11 @@
       <c r="C11" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="I11" s="46" t="s">
         <v>192</v>
-      </c>
-      <c r="I11" s="46" t="s">
-        <v>193</v>
       </c>
       <c r="J11" s="46" t="s">
         <v>23</v>
@@ -2127,16 +2135,16 @@
         <v>32</v>
       </c>
       <c r="B12" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="46" t="s">
         <v>194</v>
       </c>
-      <c r="C12" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="H12" s="46" t="s">
+      <c r="H12" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="I12" s="46" t="s">
         <v>192</v>
-      </c>
-      <c r="I12" s="46" t="s">
-        <v>193</v>
       </c>
       <c r="J12" s="46" t="s">
         <v>23</v>
@@ -2144,13 +2152,13 @@
     </row>
     <row r="13" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="C13" s="46" t="s">
         <v>197</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>198</v>
       </c>
       <c r="I13" s="46"/>
       <c r="J13" s="42" t="s">
@@ -2162,13 +2170,13 @@
     </row>
     <row r="14" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="C14" s="46" t="s">
         <v>200</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>201</v>
       </c>
       <c r="I14" s="46"/>
       <c r="J14" s="42" t="s">
@@ -2188,19 +2196,19 @@
     </row>
     <row r="16" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="C16" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="C16" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" s="46" t="s">
         <v>192</v>
-      </c>
-      <c r="I16" s="46" t="s">
-        <v>193</v>
       </c>
       <c r="L16" s="42" t="s">
         <v>43</v>
@@ -2211,13 +2219,13 @@
         <v>32</v>
       </c>
       <c r="B17" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="G17" s="42" t="s">
         <v>206</v>
-      </c>
-      <c r="G17" s="42" t="s">
-        <v>207</v>
       </c>
       <c r="H17" s="46"/>
       <c r="I17" s="46"/>
@@ -2227,10 +2235,10 @@
         <v>24</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I18" s="46"/>
       <c r="L18" s="42" t="s">
@@ -2242,19 +2250,19 @@
         <v>32</v>
       </c>
       <c r="B19" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="H19" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="I19" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="H19" s="46" t="s">
-        <v>192</v>
-      </c>
-      <c r="I19" s="46" t="s">
+      <c r="K19" s="42" t="s">
         <v>211</v>
-      </c>
-      <c r="K19" s="42" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -2262,16 +2270,16 @@
         <v>32</v>
       </c>
       <c r="B20" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="C20" s="46" t="s">
-        <v>214</v>
-      </c>
-      <c r="H20" s="46" t="s">
-        <v>192</v>
+      <c r="H20" s="52" t="s">
+        <v>256</v>
       </c>
       <c r="I20" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
@@ -2285,10 +2293,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="35" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22" s="42" t="s">
         <v>215</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>216</v>
       </c>
       <c r="I22" s="46"/>
       <c r="J22" s="42" t="s">
@@ -2303,13 +2311,13 @@
         <v>17</v>
       </c>
       <c r="B23" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C23" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="G23" s="42" t="s">
         <v>218</v>
-      </c>
-      <c r="G23" s="42" t="s">
-        <v>219</v>
       </c>
       <c r="I23" s="46"/>
       <c r="L23" s="42" t="s">
@@ -2318,16 +2326,16 @@
     </row>
     <row r="24" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="C24" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="G24" s="42" t="s">
         <v>222</v>
-      </c>
-      <c r="G24" s="42" t="s">
-        <v>223</v>
       </c>
       <c r="I24" s="46"/>
       <c r="L24" s="42" t="s">
@@ -2339,10 +2347,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L25" s="46" t="s">
         <v>34</v>
@@ -2350,13 +2358,13 @@
     </row>
     <row r="26" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="B26" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="C26" s="46" t="s">
         <v>226</v>
-      </c>
-      <c r="C26" s="46" t="s">
-        <v>227</v>
       </c>
       <c r="J26" s="46" t="s">
         <v>23</v>
@@ -2370,16 +2378,16 @@
         <v>32</v>
       </c>
       <c r="B27" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" s="46" t="s">
         <v>228</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="H27" s="46" t="s">
         <v>229</v>
       </c>
-      <c r="H27" s="46" t="s">
+      <c r="I27" s="46" t="s">
         <v>230</v>
-      </c>
-      <c r="I27" s="46" t="s">
-        <v>231</v>
       </c>
       <c r="J27" s="46" t="s">
         <v>23</v>
@@ -2390,16 +2398,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="C28" s="46" t="s">
         <v>232</v>
       </c>
-      <c r="C28" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="H28" s="46" t="s">
-        <v>192</v>
+      <c r="H28" s="52" t="s">
+        <v>256</v>
       </c>
       <c r="I28" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
@@ -2407,10 +2415,10 @@
         <v>17</v>
       </c>
       <c r="B29" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="C29" s="46" t="s">
         <v>234</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>235</v>
       </c>
       <c r="L29" s="42" t="s">
         <v>36</v>
@@ -2421,10 +2429,10 @@
         <v>17</v>
       </c>
       <c r="B30" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C30" s="46" t="s">
         <v>236</v>
-      </c>
-      <c r="C30" s="46" t="s">
-        <v>237</v>
       </c>
       <c r="L30" s="42" t="s">
         <v>36</v>
@@ -2435,10 +2443,10 @@
         <v>21</v>
       </c>
       <c r="B31" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="C31" s="46" t="s">
         <v>238</v>
-      </c>
-      <c r="C31" s="46" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
@@ -2452,10 +2460,10 @@
         <v>33</v>
       </c>
       <c r="B33" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="C33" s="46" t="s">
         <v>240</v>
-      </c>
-      <c r="C33" s="46" t="s">
-        <v>241</v>
       </c>
       <c r="J33" s="46" t="s">
         <v>23</v>
@@ -2466,10 +2474,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J34" s="46" t="s">
         <v>23</v>
@@ -2480,33 +2488,33 @@
         <v>33</v>
       </c>
       <c r="B35" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="C35" s="46" t="s">
         <v>242</v>
-      </c>
-      <c r="C35" s="46" t="s">
-        <v>243</v>
       </c>
       <c r="J35" s="46" t="s">
         <v>23</v>
       </c>
       <c r="L35" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
+        <v>250</v>
+      </c>
+      <c r="B36" s="47" t="s">
         <v>251</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="C36" s="46" t="s">
+        <v>253</v>
+      </c>
+      <c r="H36" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="L36" s="46" t="s">
         <v>252</v>
-      </c>
-      <c r="C36" s="46" t="s">
-        <v>254</v>
-      </c>
-      <c r="H36" s="46" t="s">
-        <v>250</v>
-      </c>
-      <c r="L36" s="46" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2525,11 +2533,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
@@ -2861,7 +2869,7 @@
         <v>73</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>79</v>
@@ -3478,7 +3486,7 @@
       <c r="C80" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C18"/>
+  <autoFilter ref="A1:C18" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <sortState ref="B12:C14">
     <sortCondition ref="C12:C14"/>
   </sortState>
@@ -3488,11 +3496,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3526,7 +3534,7 @@
         <v>84</v>
       </c>
       <c r="C2" s="6">
-        <v>201708161</v>
+        <v>201709251</v>
       </c>
       <c r="D2" s="48" t="s">
         <v>188</v>

</xml_diff>